<commit_message>
Cleaned up pygal code.
</commit_message>
<xml_diff>
--- a/docs/source/examples_jupyter/chemkin_io/inputs/NH3_Input_Data.xlsx
+++ b/docs/source/examples_jupyter/chemkin_io/inputs/NH3_Input_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDel Documents (Dropbox)\UDel Research\Github\pMuTT_master\docs\source\examples_jupyter\chemkin_io\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDel Documents (Dropbox)\UDel Research\Github\pMuTT_development\docs\source\examples_jupyter\chemkin_io\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6C549F-3E4D-4661-82A0-5132AA74D077}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D59E9D5-7A23-4DC1-A9CD-06A85EDBF6C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="576" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cat_sites" sheetId="4" r:id="rId1"/>
@@ -1099,7 +1099,10 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1160,10 @@
   <dimension ref="A1:BC29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:M5"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,8 +1611,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BQ60"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:T17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,8 +2644,8 @@
         <v>4</v>
       </c>
       <c r="H12" s="4">
-        <f>-20.4299999999999+0.9</f>
-        <v>-19.529999999999902</v>
+        <f>H9+1.19</f>
+        <v>-19.239999999999949</v>
       </c>
       <c r="I12" s="4">
         <v>3453.4106299999999</v>
@@ -2725,8 +2734,8 @@
         <v>4</v>
       </c>
       <c r="H13" s="4">
-        <f>-16.59+0.5</f>
-        <v>-16.09</v>
+        <f>H10+0.72</f>
+        <v>-15.869999999999974</v>
       </c>
       <c r="I13" s="4">
         <v>3426.4448400000001</v>
@@ -2809,8 +2818,8 @@
         <v>4</v>
       </c>
       <c r="H14" s="4">
-        <f>-13.21+0.3</f>
-        <v>-12.91</v>
+        <f>H11+1.28</f>
+        <v>-11.92999999999998</v>
       </c>
       <c r="I14" s="4">
         <v>1201.6048699999999</v>
@@ -2887,8 +2896,8 @@
         <v>4</v>
       </c>
       <c r="H15" s="4">
-        <f>-17.24+0.7</f>
-        <v>-16.54</v>
+        <f>H6+2.57</f>
+        <v>-14.669999999999952</v>
       </c>
       <c r="I15" s="4">
         <v>485.61399999999998</v>
@@ -4679,8 +4688,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB50E3A2-FDBB-4648-8333-2A8A81886E9C}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:B9"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>